<commit_message>
Cambie formato NA para salida a csv y genere prueba nueva. Ok
</commit_message>
<xml_diff>
--- a/series_sc/personas_mes.xlsx
+++ b/series_sc/personas_mes.xlsx
@@ -12,13 +12,13 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="123">
   <si>
     <t>Total general</t>
   </si>
@@ -372,6 +372,21 @@
   </si>
   <si>
     <t>Remuneración imponible promedio</t>
+  </si>
+  <si>
+    <t>Tasa de desempleo NENE</t>
+  </si>
+  <si>
+    <t>Tasa de desempleo ENE</t>
+  </si>
+  <si>
+    <t>Tasa de desempleo promedio ult 4 años</t>
+  </si>
+  <si>
+    <t>Tasa desempleo de activacion</t>
+  </si>
+  <si>
+    <t>2011-12</t>
   </si>
 </sst>
 </file>
@@ -3294,7 +3309,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Datos" updatedVersion="4" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Datos" updatedVersion="4" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B115" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
@@ -4051,15 +4066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -4075,8 +4088,20 @@
       <c r="E1" s="9" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -4093,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -4110,7 +4135,7 @@
         <v>110292</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -4127,7 +4152,7 @@
         <v>157156</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -4144,7 +4169,7 @@
         <v>214096</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -4161,7 +4186,7 @@
         <v>200358</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -4178,7 +4203,7 @@
         <v>198043</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -4195,7 +4220,7 @@
         <v>208509</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -4212,7 +4237,7 @@
         <v>219966</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -4229,7 +4254,7 @@
         <v>220472</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -4246,7 +4271,7 @@
         <v>232844</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -4263,7 +4288,7 @@
         <v>236635</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -4280,7 +4305,7 @@
         <v>241549</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -4297,7 +4322,7 @@
         <v>233450</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -4314,7 +4339,7 @@
         <v>222567</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -4603,7 +4628,7 @@
         <v>261007</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -4619,8 +4644,11 @@
       <c r="E33">
         <v>267734</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -4636,8 +4664,11 @@
       <c r="E34">
         <v>270459</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -4653,8 +4684,11 @@
       <c r="E35">
         <v>274902</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -4670,8 +4704,11 @@
       <c r="E36">
         <v>277615</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -4687,8 +4724,11 @@
       <c r="E37">
         <v>288745</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -4704,8 +4744,11 @@
       <c r="E38">
         <v>279798</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -4721,8 +4764,11 @@
       <c r="E39">
         <v>276114</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -4738,8 +4784,11 @@
       <c r="E40">
         <v>294264</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -4755,8 +4804,11 @@
       <c r="E41">
         <v>281497</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -4772,8 +4824,11 @@
       <c r="E42">
         <v>278848</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -4789,8 +4844,11 @@
       <c r="E43">
         <v>281105</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -4806,8 +4864,11 @@
       <c r="E44">
         <v>289223</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -4823,8 +4884,11 @@
       <c r="E45">
         <v>295655</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -4840,8 +4904,11 @@
       <c r="E46">
         <v>298253</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -4857,8 +4924,11 @@
       <c r="E47">
         <v>299881</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -4874,8 +4944,11 @@
       <c r="E48">
         <v>302208</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -4891,8 +4964,11 @@
       <c r="E49">
         <v>317208</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -4908,8 +4984,11 @@
       <c r="E50">
         <v>307911</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>7.93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -4925,8 +5004,11 @@
       <c r="E51">
         <v>303707</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -4942,8 +5024,11 @@
       <c r="E52">
         <v>322970</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -4959,8 +5044,11 @@
       <c r="E53">
         <v>307650</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -4976,8 +5064,11 @@
       <c r="E54">
         <v>305818</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -4993,8 +5084,11 @@
       <c r="E55">
         <v>309226</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -5010,8 +5104,11 @@
       <c r="E56">
         <v>313392</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>6.73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -5027,8 +5124,11 @@
       <c r="E57">
         <v>320925</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -5044,8 +5144,11 @@
       <c r="E58">
         <v>322061</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -5061,8 +5164,11 @@
       <c r="E59">
         <v>327762</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -5078,8 +5184,11 @@
       <c r="E60">
         <v>335851</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>7.04</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>51</v>
       </c>
@@ -5095,8 +5204,11 @@
       <c r="E61">
         <v>355142</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -5112,8 +5224,11 @@
       <c r="E62">
         <v>336318</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>7.72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -5129,8 +5244,11 @@
       <c r="E63">
         <v>335986</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>7.73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -5146,8 +5264,11 @@
       <c r="E64">
         <v>363107</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>7.33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -5163,8 +5284,11 @@
       <c r="E65">
         <v>346426</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>7.22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>46</v>
       </c>
@@ -5180,8 +5304,11 @@
       <c r="E66">
         <v>345153</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>45</v>
       </c>
@@ -5197,8 +5324,11 @@
       <c r="E67">
         <v>350836</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>44</v>
       </c>
@@ -5214,8 +5344,11 @@
       <c r="E68">
         <v>351512</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>43</v>
       </c>
@@ -5231,8 +5364,11 @@
       <c r="E69">
         <v>361611</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -5248,8 +5384,11 @@
       <c r="E70">
         <v>357863</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -5265,8 +5404,11 @@
       <c r="E71">
         <v>371393</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -5282,8 +5424,11 @@
       <c r="E72">
         <v>376863</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -5299,8 +5444,11 @@
       <c r="E73">
         <v>398366</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>38</v>
       </c>
@@ -5316,8 +5464,11 @@
       <c r="E74">
         <v>378073</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>37</v>
       </c>
@@ -5333,8 +5484,11 @@
       <c r="E75">
         <v>380768</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -5350,8 +5504,11 @@
       <c r="E76">
         <v>410302</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -5367,8 +5524,11 @@
       <c r="E77">
         <v>388562</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>34</v>
       </c>
@@ -5384,8 +5544,11 @@
       <c r="E78">
         <v>384854</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>33</v>
       </c>
@@ -5401,8 +5564,11 @@
       <c r="E79">
         <v>388547</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>32</v>
       </c>
@@ -5418,8 +5584,14 @@
       <c r="E80">
         <v>411542</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>10.6</v>
+      </c>
+      <c r="G80">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>31</v>
       </c>
@@ -5435,8 +5607,20 @@
       <c r="E81">
         <v>444497</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>10.9</v>
+      </c>
+      <c r="G81">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H81">
+        <v>7.7079166666666659</v>
+      </c>
+      <c r="I81">
+        <v>8.7079166666666659</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -5452,8 +5636,20 @@
       <c r="E82">
         <v>402890</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>11.4</v>
+      </c>
+      <c r="G82">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H82">
+        <v>7.74125</v>
+      </c>
+      <c r="I82">
+        <v>8.7412500000000009</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>29</v>
       </c>
@@ -5469,8 +5665,20 @@
       <c r="E83">
         <v>411101</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>11.5</v>
+      </c>
+      <c r="G83">
+        <v>10.7</v>
+      </c>
+      <c r="H83">
+        <v>7.7808333333333328</v>
+      </c>
+      <c r="I83">
+        <v>8.7808333333333337</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>28</v>
       </c>
@@ -5486,8 +5694,20 @@
       <c r="E84">
         <v>415015</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>11.6</v>
+      </c>
+      <c r="G84">
+        <v>10.8</v>
+      </c>
+      <c r="H84">
+        <v>7.822499999999998</v>
+      </c>
+      <c r="I84">
+        <v>8.822499999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -5503,8 +5723,20 @@
       <c r="E85">
         <v>435245</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>11.6</v>
+      </c>
+      <c r="G85">
+        <v>10.8</v>
+      </c>
+      <c r="H85">
+        <v>7.8683333333333323</v>
+      </c>
+      <c r="I85">
+        <v>8.8683333333333323</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -5520,8 +5752,20 @@
       <c r="E86">
         <v>408363</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>11.2</v>
+      </c>
+      <c r="G86">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H86">
+        <v>7.9120833333333325</v>
+      </c>
+      <c r="I86">
+        <v>8.9120833333333316</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>25</v>
       </c>
@@ -5537,8 +5781,20 @@
       <c r="E87">
         <v>410338</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>10.7</v>
+      </c>
+      <c r="G87">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H87">
+        <v>7.9475000000000007</v>
+      </c>
+      <c r="I87">
+        <v>8.9475000000000016</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -5554,8 +5810,20 @@
       <c r="E88">
         <v>445034</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>10.4</v>
+      </c>
+      <c r="G88">
+        <v>9.1</v>
+      </c>
+      <c r="H88">
+        <v>7.980833333333333</v>
+      </c>
+      <c r="I88">
+        <v>8.980833333333333</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>23</v>
       </c>
@@ -5571,8 +5839,20 @@
       <c r="E89">
         <v>428725</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>10</v>
+      </c>
+      <c r="G89">
+        <v>8.6</v>
+      </c>
+      <c r="H89">
+        <v>8.0120833333333348</v>
+      </c>
+      <c r="I89">
+        <v>9.0120833333333348</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -5588,8 +5868,20 @@
       <c r="E90">
         <v>423478</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G90">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H90">
+        <v>8.0474999999999994</v>
+      </c>
+      <c r="I90">
+        <v>9.0474999999999994</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>21</v>
       </c>
@@ -5605,8 +5897,20 @@
       <c r="E91">
         <v>426147</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>9.1</v>
+      </c>
+      <c r="G91">
+        <v>8.5</v>
+      </c>
+      <c r="H91">
+        <v>8.0829166666666676</v>
+      </c>
+      <c r="I91">
+        <v>9.0829166666666676</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -5622,8 +5926,17 @@
       <c r="E92">
         <v>434188</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>9</v>
+      </c>
+      <c r="H92">
+        <v>8.3662499999999991</v>
+      </c>
+      <c r="I92">
+        <v>9.3662499999999991</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -5639,8 +5952,17 @@
       <c r="E93">
         <v>436458</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>8.6</v>
+      </c>
+      <c r="H93">
+        <v>8.3891666666666662</v>
+      </c>
+      <c r="I93">
+        <v>9.3891666666666662</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -5656,8 +5978,17 @@
       <c r="E94">
         <v>437535</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H94">
+        <v>8.3954166666666676</v>
+      </c>
+      <c r="I94">
+        <v>9.3954166666666676</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -5673,8 +6004,17 @@
       <c r="E95">
         <v>441103</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>8.5</v>
+      </c>
+      <c r="H95">
+        <v>8.3683333333333341</v>
+      </c>
+      <c r="I95">
+        <v>9.3683333333333341</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -5690,8 +6030,17 @@
       <c r="E96">
         <v>442816</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H96">
+        <v>8.3891666666666662</v>
+      </c>
+      <c r="I96">
+        <v>9.3891666666666662</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -5707,8 +6056,17 @@
       <c r="E97">
         <v>474463</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H97">
+        <v>8.3789583333333351</v>
+      </c>
+      <c r="I97">
+        <v>9.3789583333333351</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -5724,8 +6082,17 @@
       <c r="E98">
         <v>447190</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>8</v>
+      </c>
+      <c r="H98">
+        <v>8.3739583333333361</v>
+      </c>
+      <c r="I98">
+        <v>9.3739583333333361</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -5741,8 +6108,17 @@
       <c r="E99">
         <v>444412</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>7.6</v>
+      </c>
+      <c r="H99">
+        <v>8.3754166666666681</v>
+      </c>
+      <c r="I99">
+        <v>9.3754166666666681</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -5758,8 +6134,17 @@
       <c r="E100">
         <v>483929</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>7.1</v>
+      </c>
+      <c r="H100">
+        <v>8.3806250000000002</v>
+      </c>
+      <c r="I100">
+        <v>9.3806250000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -5775,8 +6160,17 @@
       <c r="E101">
         <v>459466</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>7.1</v>
+      </c>
+      <c r="H101">
+        <v>8.3902083333333355</v>
+      </c>
+      <c r="I101">
+        <v>9.3902083333333355</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -5792,8 +6186,17 @@
       <c r="E102">
         <v>457084</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>7.3</v>
+      </c>
+      <c r="H102">
+        <v>8.4129166666666695</v>
+      </c>
+      <c r="I102">
+        <v>9.4129166666666695</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -5809,8 +6212,17 @@
       <c r="E103">
         <v>463711</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <v>7.3</v>
+      </c>
+      <c r="H103">
+        <v>8.4385416666666693</v>
+      </c>
+      <c r="I103">
+        <v>9.4385416666666693</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -5826,8 +6238,17 @@
       <c r="E104">
         <v>466595</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>7.3</v>
+      </c>
+      <c r="H104">
+        <v>8.4581250000000026</v>
+      </c>
+      <c r="I104">
+        <v>9.4581250000000026</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -5843,8 +6264,17 @@
       <c r="E105">
         <v>476273</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>7</v>
+      </c>
+      <c r="H105">
+        <v>8.4700000000000024</v>
+      </c>
+      <c r="I105">
+        <v>9.4700000000000024</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -5860,8 +6290,17 @@
       <c r="E106">
         <v>478624</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>7.2</v>
+      </c>
+      <c r="H106">
+        <v>8.4733333333333363</v>
+      </c>
+      <c r="I106">
+        <v>9.4733333333333363</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -5877,8 +6316,17 @@
       <c r="E107">
         <v>488588</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>7.2</v>
+      </c>
+      <c r="H107">
+        <v>8.4829166666666698</v>
+      </c>
+      <c r="I107">
+        <v>9.4829166666666698</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -5894,8 +6342,17 @@
       <c r="E108">
         <v>495712</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>7.5</v>
+      </c>
+      <c r="H108">
+        <v>8.4897916666666706</v>
+      </c>
+      <c r="I108">
+        <v>9.4897916666666706</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -5911,8 +6368,17 @@
       <c r="E109">
         <v>525267</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>7.4</v>
+      </c>
+      <c r="H109">
+        <v>8.4993750000000023</v>
+      </c>
+      <c r="I109">
+        <v>9.4993750000000023</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -5928,8 +6394,17 @@
       <c r="E110">
         <v>496939</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <v>7.4</v>
+      </c>
+      <c r="H110">
+        <v>8.4945833333333365</v>
+      </c>
+      <c r="I110">
+        <v>9.4945833333333365</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -5941,6 +6416,29 @@
       </c>
       <c r="D111">
         <v>33319</v>
+      </c>
+      <c r="F111">
+        <v>7.2</v>
+      </c>
+      <c r="H111">
+        <v>8.4879166666666688</v>
+      </c>
+      <c r="I111">
+        <v>9.4879166666666688</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>122</v>
+      </c>
+      <c r="F112">
+        <v>7.1</v>
+      </c>
+      <c r="H112">
+        <v>8.4768750000000015</v>
+      </c>
+      <c r="I112">
+        <v>9.4768750000000015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>